<commit_message>
NC92Soil - Versione 0.9 bis del 15/10/2020
- Implementata waitbar per l'importazione degli input sismici RVT
- Risolto bug relativo alla scelta casuale tra più unità GT in una singola riga che provocava un'eccezione quando la Vs era assegnata esplicitamente
</commit_message>
<xml_diff>
--- a/Stochastic input var prop.xlsx
+++ b/Stochastic input var prop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaac\Documents\Repo Git\GitLab\SRA Software\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86129A72-BA68-4046-B13F-25446BEC9CDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C8200-E7F8-4C4D-83E3-16B330BCEF9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4D2D38F4-E5D1-49A1-97A0-EF49BC19DD52}"/>
   </bookViews>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{EEA5F5C9-C08A-4F4C-B579-CCF4F14D09A9}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{EEA5F5C9-C08A-4F4C-B579-CCF4F14D09A9}">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="42">
   <si>
     <t>Unit weight
 [KN/m3]</t>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>ID3</t>
+  </si>
+  <si>
+    <t>Input files</t>
+  </si>
+  <si>
+    <t>Assign by ID</t>
+  </si>
+  <si>
+    <t>All inputs</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4957287E-A37F-4CE2-B169-A739F2ED3546}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,12 +1159,12 @@
     <col min="13" max="13" width="16.5546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="5.5546875" customWidth="1"/>
     <col min="15" max="15" width="3.5546875" customWidth="1"/>
-    <col min="16" max="16" width="19.5546875" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="19.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
@@ -1199,16 +1208,20 @@
         <v>8</v>
       </c>
       <c r="Q1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1231,19 +1244,22 @@
         <v>28</v>
       </c>
       <c r="P2">
-        <v>100</v>
-      </c>
-      <c r="Q2">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2">
         <v>7</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>15</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1262,7 +1278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1281,7 +1297,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1297,7 +1313,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +1336,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -1343,7 +1359,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -1366,7 +1382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1386,7 +1402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1396,8 +1412,17 @@
       <c r="C10" s="3">
         <v>15.3453</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
@@ -1407,8 +1432,17 @@
       <c r="C11" s="3">
         <v>15.3453</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -1418,13 +1452,25 @@
       <c r="C12" s="3">
         <v>15.3453</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
+      <c r="D13" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1433,12 +1479,18 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F68390BF-BE40-4FA6-8740-D490E73B4B13}">
           <x14:formula1>
             <xm:f>Voices!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>R2</xm:sqref>
+          <xm:sqref>S2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6FB7669-7C56-4BB5-A27E-2C28CE641A0E}">
+          <x14:formula1>
+            <xm:f>Voices!$E$1:$E$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1448,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749CBBA9-59D3-4962-B318-181DD931EBB9}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,20 +1512,26 @@
     <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>